<commit_message>
FAKER API to generate unique random test data Implemented
</commit_message>
<xml_diff>
--- a/datafiles/addEnterprise.xlsx
+++ b/datafiles/addEnterprise.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/IdeaProjects/FalconMain/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{975DDE71-B40C-9C4A-889D-E81F2F6ED96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8B0BE26-37B2-41E8-A69B-B79DFFE148DE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247E6E26-B0FC-6C44-BFDA-4DD18B546BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="10920" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10080" yWindow="10920" windowWidth="14800" windowHeight="8020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -31,44 +30,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>mYSgK</t>
-  </si>
-  <si>
-    <t>1SGpZ</t>
-  </si>
-  <si>
-    <t>DyisW</t>
-  </si>
-  <si>
-    <t>TKnzn</t>
-  </si>
-  <si>
-    <t>eYUKF</t>
-  </si>
-  <si>
-    <t>ply32</t>
-  </si>
-  <si>
-    <t>xpgxe</t>
-  </si>
-  <si>
-    <t>rf2b3</t>
-  </si>
-  <si>
-    <t>tcyfl</t>
-  </si>
-  <si>
-    <t>bokvc</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Pan</t>
+  </si>
+  <si>
+    <t>ContactPerson</t>
+  </si>
+  <si>
+    <t>ContactPersonNumber</t>
+  </si>
+  <si>
+    <t>janene</t>
+  </si>
+  <si>
+    <t>janene@mailinator.com</t>
+  </si>
+  <si>
+    <t>GORAV5967G</t>
+  </si>
+  <si>
+    <t>Dr. Domingo Ebert</t>
+  </si>
+  <si>
+    <t>9009603569</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>emailID</t>
+  </si>
+  <si>
+    <t>mobNumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,47 +455,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" customWidth="true" width="13.046875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.04296875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.2578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="26.76953125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="7" width="13" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="29">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="J5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA9B493-78C5-BD49-A440-1CB003588E17}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Error Validation Update for Kite Portal
</commit_message>
<xml_diff>
--- a/datafiles/addEnterprise.xlsx
+++ b/datafiles/addEnterprise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/IdeaProjects/FalconMain/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8013F735-2A93-4D26-B009-DA28EACE4554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{8013F735-2A93-4D26-B009-DA28EACE4554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B341EFAD-0C2E-41DA-887F-975686CC0231}"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="10920" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10080" yWindow="10920" windowWidth="14800" windowHeight="8020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -25,8 +25,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>CompanyName</t>
   </si>
@@ -51,21 +49,6 @@
     <t>ContactPersonNumber</t>
   </si>
   <si>
-    <t>janene</t>
-  </si>
-  <si>
-    <t>janene@mailinator.com</t>
-  </si>
-  <si>
-    <t>GORAV5967G</t>
-  </si>
-  <si>
-    <t>Dr. Domingo Ebert</t>
-  </si>
-  <si>
-    <t>9009603569</t>
-  </si>
-  <si>
     <t>firstName</t>
   </si>
   <si>
@@ -78,159 +61,6 @@
     <t>mobNumber</t>
   </si>
   <si>
-    <t>qww</t>
-  </si>
-  <si>
-    <t>wqw</t>
-  </si>
-  <si>
-    <t>qw</t>
-  </si>
-  <si>
-    <t>Keith</t>
-  </si>
-  <si>
-    <t>Nienow</t>
-  </si>
-  <si>
-    <t>YCZgS@mailinator.com</t>
-  </si>
-  <si>
-    <t>98260838421</t>
-  </si>
-  <si>
-    <t>Alberto</t>
-  </si>
-  <si>
-    <t>Jacobs</t>
-  </si>
-  <si>
-    <t>barnb@mailinator.com</t>
-  </si>
-  <si>
-    <t>98260431627</t>
-  </si>
-  <si>
-    <t>Denna</t>
-  </si>
-  <si>
-    <t>Lind</t>
-  </si>
-  <si>
-    <t>IWaG4@mailinator.com</t>
-  </si>
-  <si>
-    <t>98260979685</t>
-  </si>
-  <si>
-    <t>keturah</t>
-  </si>
-  <si>
-    <t>keturah@mailinator.com</t>
-  </si>
-  <si>
-    <t>GORAV9390G</t>
-  </si>
-  <si>
-    <t>Tad Medhurst</t>
-  </si>
-  <si>
-    <t>9009569766</t>
-  </si>
-  <si>
-    <t>Romeo</t>
-  </si>
-  <si>
-    <t>Adams</t>
-  </si>
-  <si>
-    <t>XatKG@mailinator.com</t>
-  </si>
-  <si>
-    <t>98260874236</t>
-  </si>
-  <si>
-    <t>kylee</t>
-  </si>
-  <si>
-    <t>kylee@mailinator.com</t>
-  </si>
-  <si>
-    <t>GORAV1721G</t>
-  </si>
-  <si>
-    <t>Isabell Conroy</t>
-  </si>
-  <si>
-    <t>9009878043</t>
-  </si>
-  <si>
-    <t>Nicky</t>
-  </si>
-  <si>
-    <t>Towne</t>
-  </si>
-  <si>
-    <t>XqePL@mailinator.com</t>
-  </si>
-  <si>
-    <t>98260902262</t>
-  </si>
-  <si>
-    <t>junita</t>
-  </si>
-  <si>
-    <t>junita@mailinator.com</t>
-  </si>
-  <si>
-    <t>GORAV4213G</t>
-  </si>
-  <si>
-    <t>Dr. Everette Treutel</t>
-  </si>
-  <si>
-    <t>9009761876</t>
-  </si>
-  <si>
-    <t>Chang</t>
-  </si>
-  <si>
-    <t>Torphy</t>
-  </si>
-  <si>
-    <t>LgvjA@mailinator.com</t>
-  </si>
-  <si>
-    <t>98260895425</t>
-  </si>
-  <si>
-    <t>shaun</t>
-  </si>
-  <si>
-    <t>shaun@mailinator.com</t>
-  </si>
-  <si>
-    <t>GORAV7973G</t>
-  </si>
-  <si>
-    <t>Tracy O'Hara</t>
-  </si>
-  <si>
-    <t>9009807315</t>
-  </si>
-  <si>
-    <t>Jene</t>
-  </si>
-  <si>
-    <t>Robel</t>
-  </si>
-  <si>
-    <t>0iemF@mailinator.com</t>
-  </si>
-  <si>
-    <t>98260655135</t>
-  </si>
-  <si>
     <t>caryn</t>
   </si>
   <si>
@@ -256,6 +86,60 @@
   </si>
   <si>
     <t>98260667881</t>
+  </si>
+  <si>
+    <t>kelley</t>
+  </si>
+  <si>
+    <t>kelley@mailinator.com</t>
+  </si>
+  <si>
+    <t>GORAV3646G</t>
+  </si>
+  <si>
+    <t>Mr. Merlin Tromp</t>
+  </si>
+  <si>
+    <t>9009765701</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>Kirlin</t>
+  </si>
+  <si>
+    <t>a52RW@mailinator.com</t>
+  </si>
+  <si>
+    <t>9826096451</t>
+  </si>
+  <si>
+    <t>denae</t>
+  </si>
+  <si>
+    <t>denae@mailinator.com</t>
+  </si>
+  <si>
+    <t>GORAV5045G</t>
+  </si>
+  <si>
+    <t>Pattie Sipes DDS</t>
+  </si>
+  <si>
+    <t>9009602328</t>
+  </si>
+  <si>
+    <t>Leonard</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>DIUuu@mailinator.com</t>
+  </si>
+  <si>
+    <t>9826080816</t>
   </si>
 </sst>
 </file>
@@ -263,7 +147,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -619,13 +503,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012C5427-1B97-4076-9064-1F6231A6FE2D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="44.25">
+    <row r="1" spans="1:5" ht="36.75" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -642,21 +526,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -668,38 +552,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA9B493-78C5-BD49-A440-1CB003588E17}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" customWidth="true" width="15.87109375" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
selenium dependency updated working on 100 user onboarding flow
</commit_message>
<xml_diff>
--- a/datafiles/addEnterprise.xlsx
+++ b/datafiles/addEnterprise.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/IdeaProjects/FalconMain/datafiles/"/>
     </mc:Choice>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="22">
   <si>
     <t>CompanyName</t>
   </si>
@@ -83,12 +83,25 @@
   </si>
   <si>
     <t>9826080816</t>
+  </si>
+  <si>
+    <t>Gary</t>
+  </si>
+  <si>
+    <t>Torphy</t>
+  </si>
+  <si>
+    <t>66S6O@mailinator.com</t>
+  </si>
+  <si>
+    <t>9826031438</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -497,7 +510,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="15.87109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" customWidth="true" width="15.87109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -516,16 +529,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change in apache poi code to get formulated data from the Workbook
</commit_message>
<xml_diff>
--- a/datafiles/addEnterprise.xlsx
+++ b/datafiles/addEnterprise.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="26">
   <si>
     <t>CompanyName</t>
   </si>
@@ -95,6 +95,18 @@
   </si>
   <si>
     <t>9826031438</t>
+  </si>
+  <si>
+    <t>Clemente</t>
+  </si>
+  <si>
+    <t>Pacocha</t>
+  </si>
+  <si>
+    <t>Xe4Eu@mailinator.com</t>
+  </si>
+  <si>
+    <t>9826098823</t>
   </si>
 </sst>
 </file>
@@ -529,16 +541,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>